<commit_message>
Added runBioSimulations code and updated file annotations.
</commit_message>
<xml_diff>
--- a/BIOMD0000000012_annotations.xlsx
+++ b/BIOMD0000000012_annotations.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/veronica_porubsky/GitHub/COMBINE_reproducible_biomodeling_workflows/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6D6433-8849-ED4C-BECF-744BA7E69F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="15960" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - Table 1_ BIOMD0000000" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1 - Table 1_ BIOMD0000000" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
   <si>
     <t>pattern</t>
   </si>
@@ -119,28 +128,18 @@
   </si>
   <si>
     <t>PZ</t>
+  </si>
+  <si>
+    <t>species</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="13"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
@@ -194,21 +193,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -219,25 +218,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ff404040"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FF404040"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -439,7 +498,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -458,7 +517,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -488,7 +547,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -514,7 +573,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -540,7 +599,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -566,7 +625,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -592,7 +651,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -618,7 +677,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -644,7 +703,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -670,7 +729,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -696,7 +755,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -709,9 +768,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -728,7 +793,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -747,7 +812,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -773,7 +838,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -799,7 +864,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -825,7 +890,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -851,7 +916,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -877,7 +942,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -903,7 +968,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -929,7 +994,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -955,7 +1020,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -981,7 +1046,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -994,9 +1059,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1010,7 +1081,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1029,7 +1100,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1059,7 +1130,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1085,7 +1156,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1111,7 +1182,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1137,7 +1208,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1163,7 +1234,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1189,7 +1260,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1215,7 +1286,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1241,7 +1312,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1267,7 +1338,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1280,316 +1351,326 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.9609" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.4609" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.3516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.3281" style="1" customWidth="1"/>
-    <col min="6" max="6" width="29.75" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="16.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="3">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="14" customHeight="1">
-      <c r="A2" t="s" s="2">
+    <row r="2" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s" s="2">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s" s="2">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s" s="2">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s" s="2">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" ht="14" customHeight="1">
-      <c r="A3" t="s" s="2">
+    <row r="3" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s" s="2">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s" s="2">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s" s="2">
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s" s="2">
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s" s="2">
+      <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" ht="14" customHeight="1">
-      <c r="A4" t="s" s="2">
+    <row r="4" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s" s="2">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s" s="2">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s" s="2">
+      <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s" s="2">
+      <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s" s="2">
+      <c r="F4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" ht="14" customHeight="1">
-      <c r="A5" t="s" s="2">
+    <row r="5" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s" s="2">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s" s="2">
+      <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s" s="2">
+      <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5" t="s" s="2">
+      <c r="E5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s" s="2">
+      <c r="F5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" ht="14" customHeight="1">
-      <c r="A6" t="s" s="2">
+    <row r="6" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s" s="2">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s" s="2">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s" s="2">
+      <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E6" t="s" s="2">
+      <c r="E6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F6" t="s" s="2">
+      <c r="F6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" ht="14" customHeight="1">
-      <c r="A7" t="s" s="2">
+    <row r="7" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s" s="2">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E7" t="s" s="2">
+      <c r="E7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F7" t="s" s="2">
+      <c r="F7" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" ht="14" customHeight="1">
-      <c r="A8" t="s" s="2">
+    <row r="8" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s" s="2">
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="s" s="2">
+      <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D8" t="s" s="2">
+      <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E8" t="s" s="2">
+      <c r="E8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F8" t="s" s="2">
+      <c r="F8" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" ht="14" customHeight="1">
-      <c r="A9" t="s" s="2">
+    <row r="9" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s" s="2">
+      <c r="B9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="s" s="2">
+      <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E9" t="s" s="2">
+      <c r="E9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F9" t="s" s="2">
+      <c r="F9" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" ht="14" customHeight="1">
-      <c r="A10" t="s" s="2">
+    <row r="10" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B10" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s" s="2">
+      <c r="B10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D10" t="s" s="2">
+      <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E10" t="s" s="2">
+      <c r="E10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F10" t="s" s="2">
+      <c r="F10" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" ht="14" customHeight="1">
-      <c r="A11" t="s" s="2">
+    <row r="11" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s" s="2">
+      <c r="B11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D11" t="s" s="2">
+      <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E11" t="s" s="2">
+      <c r="E11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F11" t="s" s="2">
+      <c r="F11" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" ht="14" customHeight="1">
-      <c r="A12" t="s" s="2">
+    <row r="12" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B12" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s" s="2">
+      <c r="B12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D12" t="s" s="2">
+      <c r="D12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E12" t="s" s="2">
+      <c r="E12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F12" t="s" s="2">
+      <c r="F12" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" ht="14" customHeight="1">
-      <c r="A13" t="s" s="2">
+    <row r="13" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B13" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s" s="2">
+      <c r="B13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D13" t="s" s="2">
+      <c r="D13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E13" t="s" s="2">
+      <c r="E13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F13" t="s" s="2">
+      <c r="F13" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" ht="14" customHeight="1">
-      <c r="A14" t="s" s="2">
+    <row r="14" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B14" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s" s="2">
+      <c r="B14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D14" t="s" s="2">
+      <c r="D14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E14" t="s" s="2">
+      <c r="E14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F14" t="s" s="2">
+      <c r="F14" s="2" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup scale="72" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>